<commit_message>
0826 add statistic parameters
</commit_message>
<xml_diff>
--- a/RobbyYu/Kmeans/Original/QS_Asia.xlsx
+++ b/RobbyYu/Kmeans/Original/QS_Asia.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20388"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\georg\PycharmProjects\pythonProject\RobbyYu\Kmeans\Original\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83FC0208-3E43-45E1-914D-E91C8357B14C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D52CBA-3052-4771-937F-4A8FAF45DE7F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" xr2:uid="{31E22BB5-03BD-43D0-8201-58162218C118}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8940" activeTab="1" xr2:uid="{31E22BB5-03BD-43D0-8201-58162218C118}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="百分比" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2030" uniqueCount="1288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2043" uniqueCount="1299">
   <si>
     <t>Year</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -3947,6 +3948,50 @@
   </si>
   <si>
     <t>National Central University</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reputation</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Scholar</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>International</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Papers per Faculty</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Citations per Faculty </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Faculty Staff with PhD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>International  Faculty</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>International Students</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>International Research Network</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Inbound Exchange</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outbound Exchange</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -3954,7 +3999,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="177" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3990,16 +4038,48 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -4007,14 +4087,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4031,10 +4194,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="2" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="3" borderId="5" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal 2" xfId="1" xr:uid="{B449C802-C1A9-43D3-BC18-F133FC275664}"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="百分比" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4348,7 +4560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76799CB-9B84-468E-A6E0-25B81C76EFF4}">
   <dimension ref="A1:V772"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="R3" sqref="R3"/>
     </sheetView>
@@ -48016,4 +48228,139 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B1A8CBB-B8F0-489A-9AB2-C297DF979E14}">
+  <dimension ref="D3:H14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="20.5" customWidth="1"/>
+    <col min="6" max="6" width="14.25" customWidth="1"/>
+    <col min="7" max="7" width="24.375" customWidth="1"/>
+    <col min="8" max="8" width="8.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="4:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D5" s="8"/>
+      <c r="F5" s="9" t="s">
+        <v>1288</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>1286</v>
+      </c>
+      <c r="H5" s="11">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F6" s="12"/>
+      <c r="G6" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D7" s="8"/>
+      <c r="F7" s="15" t="s">
+        <v>1289</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>1291</v>
+      </c>
+      <c r="H7" s="17">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D8" s="8"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="16" t="s">
+        <v>1292</v>
+      </c>
+      <c r="H8" s="17">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D9" s="8"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="16" t="s">
+        <v>1293</v>
+      </c>
+      <c r="H9" s="17">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D10" s="8"/>
+      <c r="F10" s="18" t="s">
+        <v>1290</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>1294</v>
+      </c>
+      <c r="H10" s="20">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F11" s="18"/>
+      <c r="G11" s="19" t="s">
+        <v>1295</v>
+      </c>
+      <c r="H11" s="20">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F12" s="18"/>
+      <c r="G12" s="19" t="s">
+        <v>1296</v>
+      </c>
+      <c r="H12" s="20">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F13" s="18"/>
+      <c r="G13" s="19" t="s">
+        <v>1297</v>
+      </c>
+      <c r="H13" s="20">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" ht="15.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="21"/>
+      <c r="G14" s="22" t="s">
+        <v>1298</v>
+      </c>
+      <c r="H14" s="23">
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="F10:F14"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="F5:F6"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>